<commit_message>
concerting names and recovering dropped data
</commit_message>
<xml_diff>
--- a/scrapers/scraped-data/Alpsee-Skiff-Weekend 2023_49er.xlsx
+++ b/scrapers/scraped-data/Alpsee-Skiff-Weekend 2023_49er.xlsx
@@ -497,7 +497,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -544,7 +544,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -591,7 +591,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -689,7 +689,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -736,7 +736,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -783,7 +783,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -830,7 +830,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -877,7 +877,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -924,7 +924,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -975,7 +975,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -1022,7 +1022,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -1069,7 +1069,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -1116,7 +1116,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -1167,7 +1167,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -1218,7 +1218,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -1265,7 +1265,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -1312,7 +1312,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -1359,7 +1359,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -1406,7 +1406,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -1453,7 +1453,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -1500,7 +1500,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1547,7 +1547,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1594,7 +1594,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1641,7 +1641,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1688,7 +1688,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1735,7 +1735,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1782,7 +1782,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1829,7 +1829,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1876,7 +1876,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1923,7 +1923,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1970,7 +1970,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -2017,7 +2017,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -2064,7 +2064,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -2111,7 +2111,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -2158,7 +2158,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -2205,7 +2205,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -2252,7 +2252,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -2299,7 +2299,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -2346,7 +2346,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -2393,7 +2393,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -2440,7 +2440,7 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -2487,7 +2487,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -2534,7 +2534,7 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -2581,7 +2581,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -2628,7 +2628,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -2675,7 +2675,7 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -2722,7 +2722,7 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
@@ -2769,7 +2769,7 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
@@ -2816,7 +2816,7 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
@@ -2863,7 +2863,7 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -2910,7 +2910,7 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
@@ -2957,7 +2957,7 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -3004,7 +3004,7 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
@@ -3051,7 +3051,7 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
@@ -3098,7 +3098,7 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
@@ -3145,7 +3145,7 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
@@ -3192,7 +3192,7 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -3239,7 +3239,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -3286,7 +3286,7 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
@@ -3333,7 +3333,7 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -3380,7 +3380,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
@@ -3427,7 +3427,7 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
@@ -3474,7 +3474,7 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
@@ -3521,7 +3521,7 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
@@ -3568,7 +3568,7 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
@@ -3615,7 +3615,7 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -3662,7 +3662,7 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
@@ -3709,7 +3709,7 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -3756,7 +3756,7 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -3803,7 +3803,7 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
@@ -3850,7 +3850,7 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
@@ -3897,7 +3897,7 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
@@ -3944,7 +3944,7 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
@@ -3995,7 +3995,7 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -4046,7 +4046,7 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -4093,7 +4093,7 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -4140,7 +4140,7 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -4187,7 +4187,7 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -4234,7 +4234,7 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
@@ -4281,7 +4281,7 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
@@ -4328,7 +4328,7 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
@@ -4375,7 +4375,7 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -4422,7 +4422,7 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -4469,7 +4469,7 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -4516,7 +4516,7 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -4563,7 +4563,7 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
@@ -4610,7 +4610,7 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
@@ -4657,7 +4657,7 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
@@ -4704,7 +4704,7 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
@@ -4751,7 +4751,7 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -4798,7 +4798,7 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
@@ -4849,7 +4849,7 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
@@ -4896,7 +4896,7 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
@@ -4947,7 +4947,7 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
@@ -4994,7 +4994,7 @@
         </is>
       </c>
       <c r="B97" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>
@@ -5041,7 +5041,7 @@
         </is>
       </c>
       <c r="B98" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C98" t="inlineStr">
         <is>
@@ -5088,7 +5088,7 @@
         </is>
       </c>
       <c r="B99" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C99" t="inlineStr">
         <is>
@@ -5135,7 +5135,7 @@
         </is>
       </c>
       <c r="B100" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C100" t="inlineStr">
         <is>
@@ -5186,7 +5186,7 @@
         </is>
       </c>
       <c r="B101" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C101" t="inlineStr">
         <is>
@@ -5233,7 +5233,7 @@
         </is>
       </c>
       <c r="B102" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C102" t="inlineStr">
         <is>
@@ -5280,7 +5280,7 @@
         </is>
       </c>
       <c r="B103" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C103" t="inlineStr">
         <is>
@@ -5327,7 +5327,7 @@
         </is>
       </c>
       <c r="B104" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C104" t="inlineStr">
         <is>
@@ -5374,7 +5374,7 @@
         </is>
       </c>
       <c r="B105" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C105" t="inlineStr">
         <is>
@@ -5421,7 +5421,7 @@
         </is>
       </c>
       <c r="B106" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C106" t="inlineStr">
         <is>
@@ -5468,7 +5468,7 @@
         </is>
       </c>
       <c r="B107" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C107" t="inlineStr">
         <is>
@@ -5515,7 +5515,7 @@
         </is>
       </c>
       <c r="B108" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C108" t="inlineStr">
         <is>
@@ -5562,7 +5562,7 @@
         </is>
       </c>
       <c r="B109" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C109" t="inlineStr">
         <is>
@@ -5609,7 +5609,7 @@
         </is>
       </c>
       <c r="B110" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C110" t="inlineStr">
         <is>
@@ -5656,7 +5656,7 @@
         </is>
       </c>
       <c r="B111" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C111" t="inlineStr">
         <is>
@@ -5703,7 +5703,7 @@
         </is>
       </c>
       <c r="B112" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C112" t="inlineStr">
         <is>
@@ -5750,7 +5750,7 @@
         </is>
       </c>
       <c r="B113" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C113" t="inlineStr">
         <is>
@@ -5797,7 +5797,7 @@
         </is>
       </c>
       <c r="B114" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C114" t="inlineStr">
         <is>
@@ -5844,7 +5844,7 @@
         </is>
       </c>
       <c r="B115" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C115" t="inlineStr">
         <is>
@@ -5891,7 +5891,7 @@
         </is>
       </c>
       <c r="B116" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C116" t="inlineStr">
         <is>
@@ -5942,7 +5942,7 @@
         </is>
       </c>
       <c r="B117" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C117" t="inlineStr">
         <is>
@@ -5989,7 +5989,7 @@
         </is>
       </c>
       <c r="B118" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C118" t="inlineStr">
         <is>
@@ -6036,7 +6036,7 @@
         </is>
       </c>
       <c r="B119" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C119" t="inlineStr">
         <is>
@@ -6083,7 +6083,7 @@
         </is>
       </c>
       <c r="B120" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C120" t="inlineStr">
         <is>
@@ -6130,7 +6130,7 @@
         </is>
       </c>
       <c r="B121" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C121" t="inlineStr">
         <is>
@@ -6177,7 +6177,7 @@
         </is>
       </c>
       <c r="B122" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C122" t="inlineStr">
         <is>
@@ -6224,7 +6224,7 @@
         </is>
       </c>
       <c r="B123" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C123" t="inlineStr">
         <is>
@@ -6271,7 +6271,7 @@
         </is>
       </c>
       <c r="B124" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C124" t="inlineStr">
         <is>
@@ -6318,7 +6318,7 @@
         </is>
       </c>
       <c r="B125" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C125" t="inlineStr">
         <is>
@@ -6365,7 +6365,7 @@
         </is>
       </c>
       <c r="B126" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C126" t="inlineStr">
         <is>
@@ -6416,7 +6416,7 @@
         </is>
       </c>
       <c r="B127" t="n">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="C127" t="inlineStr">
         <is>

</xml_diff>